<commit_message>
Pooh Points: normal 20260225
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-02-25.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-02-25.xlsx
@@ -434,7 +434,7 @@
     <col width="26" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
     <col width="5" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
@@ -1171,14 +1171,14 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H9" t="n">
         <v>25</v>
       </c>
       <c r="I9" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9" t="n">
         <v>7</v>
@@ -1214,10 +1214,10 @@
         <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V9" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -2975,7 +2975,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H31" t="n">
@@ -3795,7 +3795,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H41" t="n">
@@ -3877,7 +3877,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H42" t="n">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H54" t="n">
@@ -6501,14 +6501,14 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H74" t="n">
         <v>23</v>
       </c>
       <c r="I74" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J74" t="n">
         <v>4</v>
@@ -6544,10 +6544,10 @@
         <v>6</v>
       </c>
       <c r="U74" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="V74" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75">
@@ -8879,7 +8879,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H103" t="n">
@@ -9289,7 +9289,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H108" t="n">
@@ -9371,7 +9371,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H109" t="n">
@@ -9453,7 +9453,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H110" t="n">
@@ -9481,7 +9481,7 @@
         <v>4</v>
       </c>
       <c r="P110" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q110" t="n">
         <v>4</v>
@@ -10109,7 +10109,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H118" t="n">
@@ -10191,7 +10191,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H119" t="n">
@@ -10929,7 +10929,7 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H128" t="n">
@@ -10957,7 +10957,7 @@
         <v>2</v>
       </c>
       <c r="P128" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q128" t="n">
         <v>0</v>
@@ -11011,7 +11011,7 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H129" t="n">
@@ -11503,7 +11503,7 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H135" t="n">
@@ -12159,7 +12159,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>0:23 - 2OT</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H143" t="n">

</xml_diff>